<commit_message>
count value of feature5 and validate value of all feature
</commit_message>
<xml_diff>
--- a/checkValue.xlsx
+++ b/checkValue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KULIAH\SEMESTER VI\COMPUTER VISION\ViolaJones\ViolaJones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8CC39B3-09A1-492C-ADAD-525C6D833705}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9F55BBE0-D9A9-4BB1-9149-A1D19E619E7B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{13063DA0-2C6A-4A43-A6F8-A802F8E5DC4E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>s1</t>
   </si>
@@ -34,6 +34,33 @@
   </si>
   <si>
     <t>s3</t>
+  </si>
+  <si>
+    <t>4,2,16,7,3,527</t>
+  </si>
+  <si>
+    <t>3,13,6,3,2,803</t>
+  </si>
+  <si>
+    <t>5,4,11,1,4,-107</t>
+  </si>
+  <si>
+    <t>s4</t>
+  </si>
+  <si>
+    <t>5,2,4,5,1,-20</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
   </si>
 </sst>
 </file>
@@ -50,7 +77,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -60,6 +87,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -76,10 +115,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,14 +435,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984B14A6-93C2-47A9-9E0E-89D1CA1086A1}">
-  <dimension ref="B2:K6"/>
+  <dimension ref="B1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>8533</v>
@@ -521,7 +567,634 @@
         <v>803</v>
       </c>
     </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>3367</v>
+      </c>
+      <c r="C9">
+        <v>3580</v>
+      </c>
+      <c r="D9">
+        <v>3789</v>
+      </c>
+      <c r="E9">
+        <v>4003</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f>B9+E16-E9-B16</f>
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>5130</v>
+      </c>
+      <c r="C10">
+        <v>5460</v>
+      </c>
+      <c r="D10">
+        <v>5778</v>
+      </c>
+      <c r="E10">
+        <v>6101</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <f>B16+E23-E16-B23</f>
+        <v>3948</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>6555</v>
+      </c>
+      <c r="C11">
+        <v>6975</v>
+      </c>
+      <c r="D11">
+        <v>7392</v>
+      </c>
+      <c r="E11">
+        <v>7832</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <f>B23+E30-E23-B30</f>
+        <v>2530</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>7815</v>
+      </c>
+      <c r="C12">
+        <v>8294</v>
+      </c>
+      <c r="D12">
+        <v>8786</v>
+      </c>
+      <c r="E12">
+        <v>9332</v>
+      </c>
+      <c r="H12">
+        <f>H9-H10+H11</f>
+        <v>527</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>9162</v>
+      </c>
+      <c r="C13">
+        <v>9696</v>
+      </c>
+      <c r="D13">
+        <v>10246</v>
+      </c>
+      <c r="E13">
+        <v>10873</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>10448</v>
+      </c>
+      <c r="C14">
+        <v>11059</v>
+      </c>
+      <c r="D14">
+        <v>11675</v>
+      </c>
+      <c r="E14">
+        <v>12373</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>11903</v>
+      </c>
+      <c r="C15">
+        <v>12613</v>
+      </c>
+      <c r="D15">
+        <v>13313</v>
+      </c>
+      <c r="E15">
+        <v>14090</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>13879</v>
+      </c>
+      <c r="C16">
+        <v>14723</v>
+      </c>
+      <c r="D16">
+        <v>15554</v>
+      </c>
+      <c r="E16">
+        <v>16460</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>14690</v>
+      </c>
+      <c r="C17" s="4">
+        <v>15593</v>
+      </c>
+      <c r="D17" s="4">
+        <v>16490</v>
+      </c>
+      <c r="E17" s="4">
+        <v>17454</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>16551</v>
+      </c>
+      <c r="C18" s="4">
+        <v>17599</v>
+      </c>
+      <c r="D18" s="4">
+        <v>18645</v>
+      </c>
+      <c r="E18" s="4">
+        <v>19721</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>19414</v>
+      </c>
+      <c r="C19" s="4">
+        <v>20704</v>
+      </c>
+      <c r="D19" s="4">
+        <v>21986</v>
+      </c>
+      <c r="E19" s="4">
+        <v>23246</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>21893</v>
+      </c>
+      <c r="C20" s="4">
+        <v>23434</v>
+      </c>
+      <c r="D20" s="4">
+        <v>24954</v>
+      </c>
+      <c r="E20" s="4">
+        <v>26414</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>24276</v>
+      </c>
+      <c r="C21" s="4">
+        <v>26066</v>
+      </c>
+      <c r="D21" s="4">
+        <v>27803</v>
+      </c>
+      <c r="E21" s="4">
+        <v>29481</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>26674</v>
+      </c>
+      <c r="C22" s="4">
+        <v>28705</v>
+      </c>
+      <c r="D22" s="4">
+        <v>30622</v>
+      </c>
+      <c r="E22" s="4">
+        <v>32530</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>29049</v>
+      </c>
+      <c r="C23" s="4">
+        <v>31335</v>
+      </c>
+      <c r="D23" s="4">
+        <v>33423</v>
+      </c>
+      <c r="E23" s="4">
+        <v>35578</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>31379</v>
+      </c>
+      <c r="C24">
+        <v>33919</v>
+      </c>
+      <c r="D24">
+        <v>36177</v>
+      </c>
+      <c r="E24">
+        <v>38521</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>33323</v>
+      </c>
+      <c r="C25">
+        <v>36105</v>
+      </c>
+      <c r="D25">
+        <v>38524</v>
+      </c>
+      <c r="E25">
+        <v>40943</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>35122</v>
+      </c>
+      <c r="C26">
+        <v>37971</v>
+      </c>
+      <c r="D26">
+        <v>40548</v>
+      </c>
+      <c r="E26">
+        <v>43040</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>37210</v>
+      </c>
+      <c r="C27">
+        <v>40247</v>
+      </c>
+      <c r="D27">
+        <v>43032</v>
+      </c>
+      <c r="E27">
+        <v>45593</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>39272</v>
+      </c>
+      <c r="C28">
+        <v>42447</v>
+      </c>
+      <c r="D28">
+        <v>45352</v>
+      </c>
+      <c r="E28">
+        <v>47961</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>40566</v>
+      </c>
+      <c r="C29">
+        <v>43784</v>
+      </c>
+      <c r="D29">
+        <v>46759</v>
+      </c>
+      <c r="E29">
+        <v>49423</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>41811</v>
+      </c>
+      <c r="C30">
+        <v>45141</v>
+      </c>
+      <c r="D30">
+        <v>48186</v>
+      </c>
+      <c r="E30">
+        <v>50870</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>6106</v>
+      </c>
+      <c r="C34">
+        <v>6523</v>
+      </c>
+      <c r="D34">
+        <v>6946</v>
+      </c>
+      <c r="E34">
+        <v>7377</v>
+      </c>
+      <c r="F34">
+        <v>7815</v>
+      </c>
+      <c r="G34">
+        <v>8294</v>
+      </c>
+      <c r="H34">
+        <v>8786</v>
+      </c>
+      <c r="I34">
+        <v>9332</v>
+      </c>
+      <c r="J34">
+        <v>9893</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>7192</v>
+      </c>
+      <c r="C35">
+        <v>7674</v>
+      </c>
+      <c r="D35">
+        <v>8162</v>
+      </c>
+      <c r="E35">
+        <v>8658</v>
+      </c>
+      <c r="F35">
+        <v>9162</v>
+      </c>
+      <c r="G35" s="4">
+        <v>9696</v>
+      </c>
+      <c r="H35" s="4">
+        <v>10246</v>
+      </c>
+      <c r="I35" s="4">
+        <v>10873</v>
+      </c>
+      <c r="J35" s="4">
+        <v>11541</v>
+      </c>
+      <c r="L35" t="s">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <f>B34+F35-F34-B35</f>
+        <v>261</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>8204</v>
+      </c>
+      <c r="C36" s="4">
+        <v>8755</v>
+      </c>
+      <c r="D36" s="4">
+        <v>9312</v>
+      </c>
+      <c r="E36" s="4">
+        <v>9876</v>
+      </c>
+      <c r="F36" s="4">
+        <v>10448</v>
+      </c>
+      <c r="G36">
+        <v>11059</v>
+      </c>
+      <c r="H36">
+        <v>11675</v>
+      </c>
+      <c r="I36">
+        <v>12373</v>
+      </c>
+      <c r="J36">
+        <v>13128</v>
+      </c>
+      <c r="L36" t="s">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <f>F34+J35-J34-F35</f>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L37" t="s">
+        <v>2</v>
+      </c>
+      <c r="M37">
+        <f>B35+F36-F35-B36</f>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L38" t="s">
+        <v>6</v>
+      </c>
+      <c r="M38">
+        <f>F35+J36-J35-F36</f>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M39">
+        <f>M35-M36-M37+M38</f>
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>841</v>
+      </c>
+      <c r="C42">
+        <v>1064</v>
+      </c>
+      <c r="D42">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>1281</v>
+      </c>
+      <c r="C43">
+        <v>1614</v>
+      </c>
+      <c r="D43" s="4">
+        <v>1941</v>
+      </c>
+      <c r="F43" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43">
+        <f>B42+C47-C42-B47</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>1725</v>
+      </c>
+      <c r="C44">
+        <v>2170</v>
+      </c>
+      <c r="D44" s="4">
+        <v>2612</v>
+      </c>
+      <c r="F44" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44">
+        <f>C42+D47-D42-C47</f>
+        <v>534</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>2187</v>
+      </c>
+      <c r="C45">
+        <v>2758</v>
+      </c>
+      <c r="D45" s="4">
+        <v>3320</v>
+      </c>
+      <c r="F45" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45">
+        <f>B47+C52-C47-B52</f>
+        <v>545</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>2662</v>
+      </c>
+      <c r="C46">
+        <v>3358</v>
+      </c>
+      <c r="D46" s="4">
+        <v>4029</v>
+      </c>
+      <c r="F46" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46">
+        <f>C47+D52-D47-C52</f>
+        <v>499</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>3104</v>
+      </c>
+      <c r="C47">
+        <v>3887</v>
+      </c>
+      <c r="D47" s="4">
+        <v>4640</v>
+      </c>
+      <c r="G47">
+        <f>G43-G44-G45+G46</f>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>3498</v>
+      </c>
+      <c r="C48" s="4">
+        <v>4321</v>
+      </c>
+      <c r="D48" s="2">
+        <v>5131</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>3964</v>
+      </c>
+      <c r="C49" s="4">
+        <v>4850</v>
+      </c>
+      <c r="D49" s="2">
+        <v>5754</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>4251</v>
+      </c>
+      <c r="C50" s="4">
+        <v>5178</v>
+      </c>
+      <c r="D50" s="2">
+        <v>6137</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>4535</v>
+      </c>
+      <c r="C51" s="4">
+        <v>5610</v>
+      </c>
+      <c r="D51" s="2">
+        <v>6687</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>4987</v>
+      </c>
+      <c r="C52" s="4">
+        <v>6315</v>
+      </c>
+      <c r="D52" s="2">
+        <v>7567</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>